<commit_message>
Edit the XLSX test cases in order to add fifth test case
Add to cart many times
</commit_message>
<xml_diff>
--- a/MyDemoApp.xlsx
+++ b/MyDemoApp.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a81ac8ea2a7adf5/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\OneDrive\Documents\Github\mydemoapp-android-appium-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2841" documentId="8_{8BD65C4A-8675-46E8-9AA6-203A96829684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{621508EC-0295-43C4-9BC5-4F866D744109}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A96553-43BB-4559-B250-0C09544CF775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{07652D24-813E-47E9-BBAF-B7EB4B2764AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{07652D24-813E-47E9-BBAF-B7EB4B2764AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
     <sheet name="Low Level" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="199">
   <si>
     <t>Test plan</t>
   </si>
@@ -818,6 +817,24 @@
   </si>
   <si>
     <t>MDA-24</t>
+  </si>
+  <si>
+    <t>Add to cart many times</t>
+  </si>
+  <si>
+    <t>MDA-25</t>
+  </si>
+  <si>
+    <t>The number of products is displayed on the cart icon</t>
+  </si>
+  <si>
+    <t>Verify the total amount is displayed at the bottom as the number of products multiplied by the price of each product</t>
+  </si>
+  <si>
+    <t>The total amount is displayed correctly</t>
+  </si>
+  <si>
+    <t>Click on "Add to cart" button {Number} times</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1214,6 +1231,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,39 +1297,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1338,14 +1340,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1383,7 +1381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1489,7 +1487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1631,7 +1629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1639,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BB2A49-A929-4F5D-BA74-FB20428C22C8}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,10 +1653,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1673,8 +1671,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="12" t="s">
         <v>26</v>
       </c>
@@ -1689,8 +1687,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="12" t="s">
         <v>27</v>
       </c>
@@ -1703,8 +1701,8 @@
       <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="14" t="s">
         <v>28</v>
       </c>
@@ -1738,10 +1736,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="str" cm="1">
-        <f t="array" ref="A6:A29">"MDA-" &amp; _xlfn.SEQUENCE(COUNTA(C:C)-5)</f>
+        <f t="array" ref="A6:A30">"MDA-" &amp; _xlfn.SEQUENCE(COUNTA(C:C)-5)</f>
         <v>MDA-1</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="37" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1761,7 +1759,7 @@
       <c r="A7" s="20" t="str">
         <v>MDA-2</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="18" t="s">
         <v>36</v>
       </c>
@@ -1779,7 +1777,7 @@
       <c r="A8" s="20" t="str">
         <v>MDA-3</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="18" t="s">
         <v>37</v>
       </c>
@@ -1797,7 +1795,7 @@
       <c r="A9" s="20" t="str">
         <v>MDA-4</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="18" t="s">
         <v>62</v>
       </c>
@@ -1815,9 +1813,9 @@
       <c r="A10" s="20" t="str">
         <v>MDA-5</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="18" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>8</v>
@@ -1833,9 +1831,9 @@
       <c r="A11" s="20" t="str">
         <v>MDA-6</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>8</v>
@@ -1851,11 +1849,9 @@
       <c r="A12" s="20" t="str">
         <v>MDA-7</v>
       </c>
-      <c r="B12" s="33" t="s">
-        <v>38</v>
-      </c>
+      <c r="B12" s="38"/>
       <c r="C12" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>8</v>
@@ -1871,12 +1867,14 @@
       <c r="A13" s="20" t="str">
         <v>MDA-8</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="39" t="s">
+        <v>38</v>
+      </c>
       <c r="C13" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>20</v>
@@ -1889,14 +1887,12 @@
       <c r="A14" s="20" t="str">
         <v>MDA-9</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>41</v>
-      </c>
+      <c r="B14" s="40"/>
       <c r="C14" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>20</v>
@@ -1909,9 +1905,11 @@
       <c r="A15" s="20" t="str">
         <v>MDA-10</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="C15" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>8</v>
@@ -1927,9 +1925,9 @@
       <c r="A16" s="20" t="str">
         <v>MDA-11</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>8</v>
@@ -1945,11 +1943,9 @@
       <c r="A17" s="20" t="str">
         <v>MDA-12</v>
       </c>
-      <c r="B17" s="37" t="s">
-        <v>45</v>
-      </c>
+      <c r="B17" s="42"/>
       <c r="C17" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>8</v>
@@ -1965,9 +1961,11 @@
       <c r="A18" s="20" t="str">
         <v>MDA-13</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="43" t="s">
+        <v>45</v>
+      </c>
       <c r="C18" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>8</v>
@@ -1983,11 +1981,9 @@
       <c r="A19" s="20" t="str">
         <v>MDA-14</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>48</v>
-      </c>
+      <c r="B19" s="44"/>
       <c r="C19" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>8</v>
@@ -2003,9 +1999,11 @@
       <c r="A20" s="20" t="str">
         <v>MDA-15</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="29" t="s">
+        <v>48</v>
+      </c>
       <c r="C20" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>8</v>
@@ -2021,11 +2019,9 @@
       <c r="A21" s="20" t="str">
         <v>MDA-16</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>51</v>
-      </c>
+      <c r="B21" s="30"/>
       <c r="C21" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>8</v>
@@ -2041,9 +2037,11 @@
       <c r="A22" s="20" t="str">
         <v>MDA-17</v>
       </c>
-      <c r="B22" s="40"/>
+      <c r="B22" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="C22" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>8</v>
@@ -2059,12 +2057,12 @@
       <c r="A23" s="20" t="str">
         <v>MDA-18</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>20</v>
@@ -2077,9 +2075,9 @@
       <c r="A24" s="20" t="str">
         <v>MDA-19</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>7</v>
@@ -2095,12 +2093,12 @@
       <c r="A25" s="20" t="str">
         <v>MDA-20</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>20</v>
@@ -2113,11 +2111,9 @@
       <c r="A26" s="20" t="str">
         <v>MDA-21</v>
       </c>
-      <c r="B26" s="41" t="s">
-        <v>57</v>
-      </c>
+      <c r="B26" s="25"/>
       <c r="C26" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>8</v>
@@ -2133,9 +2129,11 @@
       <c r="A27" s="20" t="str">
         <v>MDA-22</v>
       </c>
-      <c r="B27" s="42"/>
+      <c r="B27" s="26" t="s">
+        <v>57</v>
+      </c>
       <c r="C27" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>8</v>
@@ -2151,12 +2149,12 @@
       <c r="A28" s="20" t="str">
         <v>MDA-23</v>
       </c>
-      <c r="B28" s="42"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>20</v>
@@ -2169,9 +2167,9 @@
       <c r="A29" s="20" t="str">
         <v>MDA-24</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>7</v>
@@ -2183,18 +2181,36 @@
         <v>8</v>
       </c>
     </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="str">
+        <v>MDA-25</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A1:B4"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D29">
+  <conditionalFormatting sqref="D6:D30">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",D6)))</formula>
     </cfRule>
@@ -2203,10 +2219,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E29" xr:uid="{FC2657C4-B913-434A-867E-9B69FBFACDA8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E30" xr:uid="{FC2657C4-B913-434A-867E-9B69FBFACDA8}">
       <formula1>"Functional,Performance,Unit,User Interface,Security, Integration, Database,Usability,User acceptance,Regression"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D29 F6:F29" xr:uid="{885C68F2-17AB-46E9-B691-4FE0F66F19B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D30 F6:F30" xr:uid="{885C68F2-17AB-46E9-B691-4FE0F66F19B4}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2220,10 +2236,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,7 +2332,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
+      <c r="A5" s="4">
         <v>1.03</v>
       </c>
       <c r="B5" s="4"/>
@@ -2333,7 +2349,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46">
+      <c r="A6" s="4">
         <v>1.04</v>
       </c>
       <c r="B6" s="4"/>
@@ -2350,7 +2366,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46">
+      <c r="A7" s="4">
         <v>1.05</v>
       </c>
       <c r="B7" s="4"/>
@@ -2359,7 +2375,7 @@
       <c r="E7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="4" t="s">
         <v>76</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -2367,7 +2383,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
+      <c r="A8" s="4">
         <v>1.06</v>
       </c>
       <c r="B8" s="4"/>
@@ -2384,11 +2400,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="46">
+      <c r="A9" s="4">
         <v>1.07</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="4"/>
@@ -2402,44 +2418,44 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="45" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>1.08</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="46">
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46">
+      <c r="A12" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B12" s="4"/>
@@ -2455,25 +2471,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="7" t="s">
         <v>170</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2486,7 +2502,7 @@
       <c r="E14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -2500,10 +2516,10 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -2517,52 +2533,52 @@
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="4" t="s">
         <v>69</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46">
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>2.0299999999999998</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>2.04</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46">
+      <c r="A19" s="4">
         <v>2.0499999999999998</v>
       </c>
       <c r="B19" s="4"/>
@@ -2579,7 +2595,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="7" t="s">
         <v>171</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2592,7 +2608,7 @@
       <c r="E20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -2600,16 +2616,16 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46">
+      <c r="A21" s="4">
         <v>3.01</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -2617,16 +2633,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="46">
+      <c r="A22" s="4">
         <v>3.02</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="4" t="s">
         <v>69</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -2634,16 +2650,16 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46">
+      <c r="A23" s="4">
         <v>3.03</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -2651,16 +2667,16 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+      <c r="A24" s="4">
         <v>3.04</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -2668,7 +2684,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="46">
+      <c r="A25" s="4">
         <v>3.05</v>
       </c>
       <c r="B25" s="4"/>
@@ -2685,7 +2701,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="7" t="s">
         <v>172</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2698,7 +2714,7 @@
       <c r="E26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="47" t="s">
+      <c r="F26" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -2712,10 +2728,10 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -2729,44 +2745,44 @@
       <c r="B28" s="4"/>
       <c r="C28" s="10"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="4" t="s">
         <v>69</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46">
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>4.03</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46">
+      <c r="A30" s="4">
         <v>4.04</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -2774,16 +2790,16 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="46">
+      <c r="A31" s="4">
         <v>4.05</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="F31" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -2791,11 +2807,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="7" t="s">
         <v>173</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
@@ -2804,7 +2820,7 @@
       <c r="E32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="47" t="s">
+      <c r="F32" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -2812,119 +2828,113 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46">
+      <c r="A33" s="4">
         <v>5.01</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>5.0199999999999996</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>97</v>
+      <c r="E34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46">
+      <c r="A35" s="4">
         <v>5.03</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="46" t="s">
-        <v>99</v>
+      <c r="E35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G36" s="7" t="s">
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>5.04</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>6.01</v>
+        <v>5.05</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>6.02</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="4" t="s">
-        <v>169</v>
-      </c>
+      <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>102</v>
+        <v>196</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="47" t="s">
-        <v>175</v>
+      <c r="A39" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
@@ -2933,7 +2943,7 @@
       <c r="E39" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="47" t="s">
+      <c r="F39" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G39" s="7" t="s">
@@ -2942,474 +2952,480 @@
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>7.01</v>
+        <v>6.01</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>7.02</v>
+        <v>6.02</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46">
-        <v>7.03</v>
+      <c r="A42" s="4">
+        <v>6.03</v>
       </c>
       <c r="B42" s="4"/>
-      <c r="C42" s="48" t="s">
-        <v>115</v>
-      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="46">
-        <v>7.04</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="46">
-        <v>7.05</v>
+      <c r="A43" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>7.01</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="s">
+    <row r="45" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>7.02</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
+      <c r="B46" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E46" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="47" t="s">
+      <c r="F46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>8.01</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>8.02</v>
+        <v>8.01</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="46" t="s">
+      <c r="E47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>8.02</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F47" s="46" t="s">
+      <c r="F48" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="46">
+      <c r="G48" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>8.0299999999999994</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="F48" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="46">
-        <v>8.0399999999999991</v>
-      </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="C49" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="4">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7" t="s">
+      <c r="B52" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E52" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F50" s="47" t="s">
+      <c r="F52" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G50" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="G52" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>9.01</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>9.02</v>
-      </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F52" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="46">
-        <v>9.0299999999999994</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>122</v>
+        <v>104</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F54" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G54" s="7" t="s">
+    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>9.02</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>10.01</v>
+        <v>9.0299999999999994</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="D55" s="4"/>
-      <c r="E55" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>105</v>
+      <c r="E55" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>10.02</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" s="46" t="s">
-        <v>120</v>
+      <c r="E56" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="46">
-        <v>10.029999999999999</v>
-      </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="F57" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="G57" s="4" t="s">
+    <row r="57" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46">
-        <v>10.039999999999999</v>
+      <c r="A58" s="4">
+        <v>10.01</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>124</v>
+        <v>104</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F59" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G59" s="7" t="s">
+    <row r="59" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>10.02</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>11.01</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F60" s="45" t="s">
-        <v>105</v>
+      <c r="E60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>11.02</v>
-      </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="F61" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="G61" s="4" t="s">
+    <row r="61" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G61" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="46">
-        <v>11.03</v>
+      <c r="A62" s="4">
+        <v>11.01</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="F62" s="46" t="s">
-        <v>122</v>
+      <c r="E62" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="46">
-        <v>11.04</v>
+      <c r="A63" s="4">
+        <v>11.02</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="F63" s="46" t="s">
-        <v>126</v>
+      <c r="E63" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="46">
-        <v>11.05</v>
+      <c r="A64" s="4">
+        <v>11.03</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="46">
-        <v>11.06</v>
+      <c r="A65" s="4">
+        <v>11.04</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="47" t="s">
+      <c r="A66" s="7" t="s">
         <v>180</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
@@ -3418,7 +3434,7 @@
       <c r="E66" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F66" s="47" t="s">
+      <c r="F66" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G66" s="7" t="s">
@@ -3432,10 +3448,10 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="46" t="s">
+      <c r="E67" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F67" s="45" t="s">
+      <c r="F67" s="3" t="s">
         <v>105</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -3449,68 +3465,62 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="F68" s="46" t="s">
-        <v>132</v>
+      <c r="E68" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="46">
+      <c r="A69" s="4">
         <v>12.03</v>
       </c>
       <c r="B69" s="4"/>
-      <c r="C69" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F70" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G70" s="7" t="s">
+    <row r="70" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>12.04</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>13.01</v>
+        <v>12.05</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F71" s="45" t="s">
-        <v>105</v>
+      <c r="E71" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>14</v>
@@ -3518,71 +3528,71 @@
     </row>
     <row r="72" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>13.02</v>
+        <v>12.06</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-      <c r="E72" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="F72" s="46" t="s">
-        <v>132</v>
+      <c r="E72" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="46">
-        <v>13.03</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7" t="s">
+    <row r="73" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E73" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F74" s="47" t="s">
+      <c r="F73" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="G73" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>14.01</v>
+        <v>13.02</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
-      <c r="E75" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F75" s="45" t="s">
-        <v>105</v>
+      <c r="E75" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>14</v>
@@ -3590,898 +3600,1027 @@
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>14.02</v>
+        <v>13.03</v>
       </c>
       <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="8"/>
+      <c r="C76" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="46">
-        <v>14.03</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G77" s="4" t="s">
+    <row r="77" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G77" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="46">
-        <v>14.04</v>
+      <c r="A78" s="4">
+        <v>14.01</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>143</v>
+        <v>104</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="47" t="s">
+    <row r="79" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>14.02</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>14.03</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7" t="s">
+      <c r="B81" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="E81" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F79" s="47" t="s">
+      <c r="F81" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G79" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="G81" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
         <v>15.01</v>
       </c>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="46" t="s">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F80" s="45" t="s">
+      <c r="F82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G80" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="G82" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
         <v>15.02</v>
       </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="46" t="s">
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F81" s="46" t="s">
+      <c r="F83" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="46">
-        <v>15.03</v>
-      </c>
-      <c r="B82" s="46"/>
-      <c r="C82" s="46"/>
-      <c r="D82" s="48"/>
-      <c r="E82" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="F82" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="G82" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F83" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G83" s="7" t="s">
+      <c r="G83" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
+        <v>15.03</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>15.04</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
         <v>16.010000000000002</v>
       </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4" t="s">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>16.02</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>16.03</v>
+      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E84" s="46" t="s">
+      <c r="E91" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F84" s="46" t="s">
+      <c r="F91" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="46">
-        <v>16.02</v>
-      </c>
-      <c r="B85" s="46"/>
-      <c r="C85" s="46"/>
-      <c r="D85" s="46"/>
-      <c r="E85" s="46" t="s">
+      <c r="G91" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>17.02</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F85" s="46" t="s">
+      <c r="F92" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G85" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="46">
-        <v>16.03</v>
-      </c>
-      <c r="B86" s="46"/>
-      <c r="C86" s="48" t="s">
+      <c r="G92" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>17.03</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D86" s="46"/>
-      <c r="E86" s="46" t="s">
+      <c r="D93" s="4"/>
+      <c r="E93" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F86" s="46" t="s">
+      <c r="F93" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G86" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="46">
-        <v>16.04</v>
-      </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4">
+      <c r="G93" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>17.04</v>
+      </c>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4">
         <v>10203040</v>
       </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="46" t="s">
+      <c r="D94" s="8"/>
+      <c r="E94" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F87" s="46" t="s">
+      <c r="F94" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G87" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="46">
-        <v>16.05</v>
-      </c>
-      <c r="B88" s="46"/>
-      <c r="C88" s="46"/>
-      <c r="D88" s="48"/>
-      <c r="E88" s="46" t="s">
+      <c r="G94" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>17.05</v>
+      </c>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F88" s="46" t="s">
+      <c r="F95" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G88" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="G95" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7" t="s">
+      <c r="C96" s="7"/>
+      <c r="D96" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E89" s="7" t="s">
+      <c r="E96" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F89" s="47" t="s">
+      <c r="F96" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G89" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>17.010000000000002</v>
-      </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F90" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="46">
-        <v>17.02</v>
-      </c>
-      <c r="B91" s="46"/>
-      <c r="C91" s="46"/>
-      <c r="D91" s="46"/>
-      <c r="E91" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="F91" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="G91" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="46">
-        <v>17.03</v>
-      </c>
-      <c r="B92" s="46"/>
-      <c r="C92" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="D92" s="46"/>
-      <c r="E92" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="F92" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="46">
-        <v>17.04</v>
-      </c>
-      <c r="B93" s="46"/>
-      <c r="C93" s="46">
-        <v>10203040</v>
-      </c>
-      <c r="D93" s="46"/>
-      <c r="E93" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="F93" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="G93" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="46">
-        <v>17.05</v>
-      </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="46"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="F94" s="46" t="s">
-        <v>153</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F95" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G95" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>18.010000000000002</v>
-      </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="F96" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="G96" s="4" t="s">
+      <c r="G96" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
-        <v>18.02</v>
+        <v>18.010000000000002</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="46" t="s">
+      <c r="D97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>18.02</v>
+      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F97" s="46" t="s">
+      <c r="F98" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G97" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="46">
+      <c r="G98" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
         <v>18.03</v>
       </c>
-      <c r="B98" s="46"/>
-      <c r="C98" s="46">
+      <c r="B99" s="4"/>
+      <c r="C99" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>18.04</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4">
         <v>10203040</v>
       </c>
-      <c r="D98" s="48"/>
-      <c r="E98" s="46" t="s">
+      <c r="D100" s="4"/>
+      <c r="E100" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F98" s="46" t="s">
+      <c r="F100" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G98" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="46">
-        <v>18.04</v>
-      </c>
-      <c r="B99" s="46"/>
-      <c r="C99" s="46"/>
-      <c r="D99" s="48"/>
-      <c r="E99" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="F99" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="G99" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F100" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G100" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
-        <v>19.010000000000002</v>
+        <v>18.05</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="46" t="s">
+      <c r="D101" s="8"/>
+      <c r="E101" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F101" s="46" t="s">
+      <c r="F103" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G101" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="46">
+      <c r="G103" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
         <v>19.02</v>
-      </c>
-      <c r="B102" s="46"/>
-      <c r="C102" s="46"/>
-      <c r="D102" s="46"/>
-      <c r="E102" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="F102" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="G102" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="46">
-        <v>19.03</v>
-      </c>
-      <c r="B103" s="46"/>
-      <c r="C103" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="D103" s="46"/>
-      <c r="E103" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="F103" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G103" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="46">
-        <v>19.04</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="8"/>
-      <c r="E104" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="F104" s="46" t="s">
-        <v>155</v>
+      <c r="E104" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E105" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F105" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>19.03</v>
+      </c>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4">
+        <v>10203040</v>
+      </c>
+      <c r="D105" s="8"/>
+      <c r="E105" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
-        <v>20.010000000000002</v>
+        <v>19.04</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="46" t="s">
+      <c r="D106" s="8"/>
+      <c r="E106" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F106" s="46" t="s">
+      <c r="F108" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G106" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="46">
+      <c r="G108" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
         <v>20.02</v>
       </c>
-      <c r="B107" s="46"/>
-      <c r="C107" s="46"/>
-      <c r="D107" s="46"/>
-      <c r="E107" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="F107" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="G107" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="46">
-        <v>20.03</v>
-      </c>
-      <c r="B108" s="46"/>
-      <c r="C108" s="46"/>
-      <c r="D108" s="46"/>
-      <c r="E108" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="F108" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="G108" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F109" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G109" s="7" t="s">
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G109" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
+        <v>20.03</v>
+      </c>
+      <c r="B110" s="4"/>
+      <c r="C110" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>20.04</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
         <v>21.01</v>
       </c>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="46" t="s">
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F110" s="46" t="s">
+      <c r="F113" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G110" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="46">
-        <v>21.02</v>
-      </c>
-      <c r="B111" s="46"/>
-      <c r="C111" s="46"/>
-      <c r="D111" s="46"/>
-      <c r="E111" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F111" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="G111" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="46">
-        <v>21.03</v>
-      </c>
-      <c r="B112" s="46"/>
-      <c r="C112" s="46"/>
-      <c r="D112" s="46"/>
-      <c r="E112" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="F112" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="G112" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C113" s="7"/>
-      <c r="D113" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F113" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G113" s="7" t="s">
+      <c r="G113" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
-        <v>22.01</v>
+        <v>21.02</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
-      <c r="E114" s="46" t="s">
+      <c r="E114" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>21.03</v>
+      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>22.01</v>
+      </c>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F114" s="46" t="s">
+      <c r="F117" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G114" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="46">
-        <v>22.02</v>
-      </c>
-      <c r="B115" s="46"/>
-      <c r="C115" s="46"/>
-      <c r="D115" s="46"/>
-      <c r="E115" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F115" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="G115" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="46">
-        <v>22.03</v>
-      </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="46" t="s">
-        <v>163</v>
-      </c>
-      <c r="F116" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="G116" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C117" s="7"/>
-      <c r="D117" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E117" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F117" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G117" s="7" t="s">
+      <c r="G117" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
-        <v>23.01</v>
+        <v>22.02</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
-      <c r="E118" s="46" t="s">
+      <c r="E118" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>22.03</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C120" s="7"/>
+      <c r="D120" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>23.01</v>
+      </c>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F118" s="46" t="s">
+      <c r="F121" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G118" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="46">
-        <v>23.02</v>
-      </c>
-      <c r="B119" s="46"/>
-      <c r="C119" s="46"/>
-      <c r="D119" s="46"/>
-      <c r="E119" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F119" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="G119" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="46">
-        <v>23.03</v>
-      </c>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="F120" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F121" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G121" s="7" t="s">
+      <c r="G121" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
-        <v>24.01</v>
+        <v>23.02</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
-      <c r="E122" s="46" t="s">
+      <c r="E122" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <v>23.03</v>
+      </c>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <v>24.01</v>
+      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F122" s="46" t="s">
+      <c r="F125" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G122" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="46">
+      <c r="G125" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
         <v>24.02</v>
       </c>
-      <c r="B123" s="46"/>
-      <c r="C123" s="46"/>
-      <c r="D123" s="46"/>
-      <c r="E123" s="46" t="s">
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F123" s="46" t="s">
+      <c r="F126" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G123" s="46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="46">
+      <c r="G126" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
         <v>24.03</v>
       </c>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="46" t="s">
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G128" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>25.01</v>
+      </c>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>25.02</v>
+      </c>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>25.03</v>
+      </c>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="8"/>
+      <c r="E131" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F124" s="46" t="s">
+      <c r="F131" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G124" s="4" t="s">
+      <c r="G131" s="4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C42" r:id="rId1" xr:uid="{64AF72A0-1176-4FC2-82F5-9445129298DA}"/>
-    <hyperlink ref="C86" r:id="rId2" xr:uid="{4DA03095-1165-4145-95A0-BEDD2B75ABEF}"/>
-    <hyperlink ref="C103" r:id="rId3" xr:uid="{22FA6C18-51D9-4FC5-887D-778470AC23D2}"/>
-    <hyperlink ref="C92" r:id="rId4" xr:uid="{2787B926-0A11-47E1-9928-11316AAC06CE}"/>
+    <hyperlink ref="C49" r:id="rId1" xr:uid="{64AF72A0-1176-4FC2-82F5-9445129298DA}"/>
+    <hyperlink ref="C93" r:id="rId2" xr:uid="{4DA03095-1165-4145-95A0-BEDD2B75ABEF}"/>
+    <hyperlink ref="C110" r:id="rId3" xr:uid="{22FA6C18-51D9-4FC5-887D-778470AC23D2}"/>
+    <hyperlink ref="C99" r:id="rId4" xr:uid="{2787B926-0A11-47E1-9928-11316AAC06CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>